<commit_message>
Vref to Internal GAM and GPS module to turn off or on in Message.cpp Digit display in debug mode
</commit_message>
<xml_diff>
--- a/Daten/Akku LIPO.xlsx
+++ b/Daten/Akku LIPO.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t xml:space="preserve">// Calcul des coefficients de mesures en fonction des resistances </t>
   </si>
@@ -36,23 +36,50 @@
     <t>COEF</t>
   </si>
   <si>
-    <t>volt</t>
-  </si>
-  <si>
-    <t>digit</t>
-  </si>
-  <si>
-    <t>erechnet software</t>
+    <t>// VREF = 1,1V (reference interne) 1,1/1024=0.0010742</t>
+  </si>
+  <si>
+    <t>messen</t>
+  </si>
+  <si>
+    <t>ablesen debug</t>
+  </si>
+  <si>
+    <t>eintragen</t>
+  </si>
+  <si>
+    <t>Lipo Spannung</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
+    <t>4S</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>Vref/Digit</t>
+  </si>
+  <si>
+    <t>Digit</t>
+  </si>
+  <si>
+    <t>Lipo Digit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,7 +110,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -91,11 +118,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -169,6 +201,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -203,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -378,233 +412,299 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>B6/B7</f>
+        <v>1.0742187500000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8">
-        <f>A6/A7</f>
-        <v>4.8828125E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.83</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <f>B8/(B11/(A11+B11))</f>
+        <v>5.1884765625000006E-3</v>
+      </c>
+      <c r="F11">
+        <v>4.1740000000000004</v>
+      </c>
+      <c r="G11" s="2">
+        <f>F11</f>
+        <v>4.1740000000000004</v>
+      </c>
+      <c r="H11">
+        <v>821</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <f>G11/H11</f>
+        <v>5.084043848964678E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.87</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <f>B8/(B12/(A12+B12))</f>
+        <v>9.5283203125000032E-3</v>
+      </c>
+      <c r="F12">
+        <v>4.1890000000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <f>F12+F11</f>
+        <v>8.3629999999999995</v>
+      </c>
+      <c r="H12">
+        <v>888</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <f t="shared" ref="J12:J14" si="0">G12/H12</f>
+        <v>9.4177927927927927E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11.8</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <f>B8/(B13/(A13+B13))</f>
+        <v>1.3750000000000002E-2</v>
+      </c>
+      <c r="F13">
+        <v>4.173</v>
+      </c>
+      <c r="G13" s="2">
+        <f>F13+F12+F11</f>
+        <v>12.536000000000001</v>
+      </c>
+      <c r="H13">
+        <v>940</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3336170212765959E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15.8</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B8/(B14/(A14+B14))</f>
+        <v>1.8046875000000004E-2</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>7</v>
       </c>
-      <c r="J10" t="s">
+      <c r="H16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="B11">
-        <v>3.83</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <f>A8/(C11/(B11+C11))</f>
-        <v>2.3583984375000002E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="G11">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="H11">
-        <f>F11/G11</f>
-        <v>177.5616</v>
-      </c>
-      <c r="J11">
-        <f>H11*D11</f>
-        <v>4.1876100000000003</v>
-      </c>
-      <c r="L11">
-        <v>4.17</v>
-      </c>
-      <c r="M11" s="2">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="O11" s="1">
-        <f>L11/M11</f>
-        <v>1.0270935960591134</v>
-      </c>
-      <c r="P11" s="1">
-        <f>O11*D11</f>
-        <v>2.4222959321120695E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="B12">
-        <v>7.87</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <f>A8/(C12/(B12+C12))</f>
-        <v>4.3310546875000008E-2</v>
-      </c>
-      <c r="F12">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="G12">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ref="H12:H14" si="0">F12/G12</f>
-        <v>189.03040000000001</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12:J14" si="1">H12*D12</f>
-        <v>8.1870100000000026</v>
-      </c>
-      <c r="L12">
-        <v>8.35</v>
-      </c>
-      <c r="M12" s="2">
-        <v>7.95</v>
-      </c>
-      <c r="O12" s="1">
-        <f t="shared" ref="O12:O14" si="2">L12/M12</f>
-        <v>1.050314465408805</v>
-      </c>
-      <c r="P12" s="1">
-        <f t="shared" ref="P12:P14" si="3">O12*D12</f>
-        <v>4.5489693887578626E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="B13">
-        <v>11.8</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <f>A8/(C13/(B13+C13))</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="G13">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>200.4992</v>
-      </c>
-      <c r="J13">
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>4.181</v>
+      </c>
+      <c r="G18" s="2">
+        <f>F18</f>
+        <v>4.181</v>
+      </c>
+      <c r="H18">
+        <v>842</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <f>G18/H18</f>
+        <v>4.9655581947743469E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="G19" s="2">
+        <f>F19+F18</f>
+        <v>8.3650000000000002</v>
+      </c>
+      <c r="H19">
+        <v>895</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <f t="shared" ref="J19:J21" si="1">G19/H19</f>
+        <v>9.3463687150837985E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>4.1909999999999998</v>
+      </c>
+      <c r="G20" s="2">
+        <f>F20+F19+F18</f>
+        <v>12.556000000000001</v>
+      </c>
+      <c r="H20">
+        <v>949</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
         <f t="shared" si="1"/>
-        <v>12.5312</v>
-      </c>
-      <c r="L13">
-        <v>12.53</v>
-      </c>
-      <c r="M13" s="2">
-        <v>12.16</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0304276315789473</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="3"/>
-        <v>6.4401726973684209E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="B14">
-        <v>15.8</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <f>A8/(C14/(B14+C14))</f>
-        <v>8.203125E-2</v>
-      </c>
-      <c r="F14">
-        <v>0.99</v>
-      </c>
-      <c r="G14">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>202.75200000000001</v>
-      </c>
-      <c r="J14">
+        <v>1.3230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>4.181</v>
+      </c>
+      <c r="G21" s="2">
+        <f>F21+F20+F19+F18</f>
+        <v>16.737000000000002</v>
+      </c>
+      <c r="H21">
+        <v>960</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1">
         <f t="shared" si="1"/>
-        <v>16.632000000000001</v>
-      </c>
-      <c r="L14">
-        <v>16.7</v>
-      </c>
-      <c r="M14" s="2">
-        <v>16.079999999999998</v>
-      </c>
-      <c r="O14" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0385572139303483</v>
-      </c>
-      <c r="P14" s="1">
-        <f t="shared" si="3"/>
-        <v>8.5194146455223885E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="M15" s="2"/>
+        <v>1.7434375000000002E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -613,24 +713,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gps_alt_m changed from uint8_t to uint16_t Added Excel file LIOP 3S
</commit_message>
<xml_diff>
--- a/Daten/Akku LIPO.xlsx
+++ b/Daten/Akku LIPO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935"/>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -75,11 +75,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,10 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -127,7 +129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -201,7 +203,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -236,7 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -412,44 +412,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -457,7 +457,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -465,7 +465,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -474,7 +474,7 @@
         <v>1.0742187500000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="F9" t="s">
         <v>7</v>
       </c>
@@ -485,7 +485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>3.83</v>
       </c>
@@ -522,23 +522,23 @@
         <f>B8/(B11/(A11+B11))</f>
         <v>5.1884765625000006E-3</v>
       </c>
-      <c r="F11">
-        <v>4.1740000000000004</v>
+      <c r="F11" s="3">
+        <v>4.1669999999999998</v>
       </c>
       <c r="G11" s="2">
         <f>F11</f>
-        <v>4.1740000000000004</v>
+        <v>4.1669999999999998</v>
       </c>
       <c r="H11">
-        <v>821</v>
+        <v>828</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
         <f>G11/H11</f>
-        <v>5.084043848964678E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.0326086956521739E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>7.87</v>
       </c>
@@ -549,23 +549,23 @@
         <f>B8/(B12/(A12+B12))</f>
         <v>9.5283203125000032E-3</v>
       </c>
-      <c r="F12">
-        <v>4.1890000000000001</v>
+      <c r="F12" s="3">
+        <v>4.1740000000000004</v>
       </c>
       <c r="G12" s="2">
         <f>F12+F11</f>
-        <v>8.3629999999999995</v>
+        <v>8.3410000000000011</v>
       </c>
       <c r="H12">
-        <v>888</v>
+        <v>894</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1">
-        <f t="shared" ref="J12:J14" si="0">G12/H12</f>
-        <v>9.4177927927927927E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J12:J13" si="0">G12/H12</f>
+        <v>9.3299776286353484E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>11.8</v>
       </c>
@@ -576,23 +576,23 @@
         <f>B8/(B13/(A13+B13))</f>
         <v>1.3750000000000002E-2</v>
       </c>
-      <c r="F13">
-        <v>4.173</v>
+      <c r="F13" s="3">
+        <v>4.1710000000000003</v>
       </c>
       <c r="G13" s="2">
         <f>F13+F12+F11</f>
-        <v>12.536000000000001</v>
+        <v>12.512</v>
       </c>
       <c r="H13">
-        <v>940</v>
+        <v>946</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>1.3336170212765959E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.3226215644820296E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>15.8</v>
       </c>
@@ -607,10 +607,10 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="F16" t="s">
         <v>7</v>
       </c>
@@ -621,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10">
       <c r="E17" t="s">
         <v>13</v>
       </c>
@@ -638,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10">
       <c r="F18">
         <v>4.181</v>
       </c>
@@ -655,7 +655,7 @@
         <v>4.9655581947743469E-3</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10">
       <c r="F19">
         <v>4.1840000000000002</v>
       </c>
@@ -672,7 +672,7 @@
         <v>9.3463687150837985E-3</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10">
       <c r="F20">
         <v>4.1909999999999998</v>
       </c>
@@ -689,7 +689,7 @@
         <v>1.3230769230769232E-2</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10">
       <c r="F21">
         <v>4.181</v>
       </c>
@@ -713,24 +713,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>